<commit_message>
BaoCaoTongHop: Add DatVe, ThuChi
</commit_message>
<xml_diff>
--- a/storage/app/reports/bao-cao-tong-hop.xlsx
+++ b/storage/app/reports/bao-cao-tong-hop.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Công nợ" sheetId="1" r:id="rId1"/>
@@ -76,6 +76,7 @@
     <definedName name="NHAP_XT" localSheetId="2">#REF!</definedName>
     <definedName name="NHAP_XT" localSheetId="4">#REF!</definedName>
     <definedName name="NHAP_XT">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Công nợ'!$A$1:$F$11</definedName>
     <definedName name="PHIEU_NX">'[2]NHAP LIEU'!$D$7:$D$250</definedName>
     <definedName name="SL_152">[1]Nhập_xuất!$P$6:$P$101</definedName>
     <definedName name="TEN">'[2]TÊN KH'!$B$3:$L$69</definedName>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
   <si>
     <t>STT</t>
   </si>
@@ -209,10 +210,10 @@
     <t>Nơi đến</t>
   </si>
   <si>
-    <t>Số dư</t>
+    <t>Đầu kỳ</t>
   </si>
   <si>
-    <t>Đầu kỳ</t>
+    <t>Còn dư</t>
   </si>
 </sst>
 </file>
@@ -340,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -441,30 +442,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="hair">
         <color indexed="64"/>
@@ -476,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -535,16 +512,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -565,7 +536,7 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -584,12 +555,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -634,6 +599,48 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 4" xfId="1"/>
@@ -641,6 +648,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -13319,7 +13394,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="2E353D"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -13577,82 +13652,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="15" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="10" style="14" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="15" customWidth="1"/>
+    <col min="5" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="46"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="50"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="46"/>
     </row>
     <row r="6" spans="1:6" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
@@ -13663,192 +13734,192 @@
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="46"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="50"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="46"/>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="D45" s="4"/>
     </row>
@@ -13858,58 +13929,61 @@
     <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="18.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="49" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="16" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="16" customWidth="1"/>
     <col min="4" max="4" width="16" style="16" customWidth="1"/>
     <col min="5" max="5" width="18" style="16" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="16" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="16"/>
+    <col min="7" max="8" width="9.140625" style="16" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="16" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="16"/>
+    <col min="10" max="11" width="9.140625" style="16" customWidth="1"/>
     <col min="12" max="15" width="13.7109375" style="16" customWidth="1"/>
-    <col min="16" max="18" width="12.5703125" style="16" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="16"/>
+    <col min="16" max="17" width="12.5703125" style="16" customWidth="1"/>
+    <col min="18" max="18" width="0" style="16" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
     </row>
-    <row r="2" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -13956,57 +14030,52 @@
         <v>21</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="22"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="18"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="18"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="24"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -14021,16 +14090,15 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="19"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="21"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14039,49 +14107,49 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:N6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="18.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="49" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="16" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="16" customWidth="1"/>
     <col min="4" max="4" width="16" style="16" customWidth="1"/>
     <col min="5" max="5" width="18" style="16" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="16" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="16"/>
+    <col min="7" max="8" width="9.140625" style="16" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="16" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="16"/>
+    <col min="10" max="11" width="9.140625" style="16" customWidth="1"/>
     <col min="12" max="15" width="13.7109375" style="16" customWidth="1"/>
-    <col min="16" max="18" width="12.5703125" style="16" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="16"/>
+    <col min="16" max="17" width="12.5703125" style="16" customWidth="1"/>
+    <col min="18" max="18" width="0" style="16" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
     </row>
-    <row r="2" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -14128,57 +14196,52 @@
         <v>21</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="22"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="18"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="18"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="24"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -14193,13 +14256,12 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="19"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="21"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14211,49 +14273,49 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:N6"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="18.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="49" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="16" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="16" customWidth="1"/>
     <col min="4" max="4" width="16" style="16" customWidth="1"/>
     <col min="5" max="5" width="18" style="16" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="16" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="16"/>
+    <col min="7" max="8" width="9.140625" style="16" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="16" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="16"/>
+    <col min="10" max="11" width="9.140625" style="16" customWidth="1"/>
     <col min="12" max="15" width="13.7109375" style="16" customWidth="1"/>
-    <col min="16" max="18" width="12.5703125" style="16" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="16"/>
+    <col min="16" max="17" width="12.5703125" style="16" customWidth="1"/>
+    <col min="18" max="18" width="0" style="16" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
     </row>
-    <row r="2" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -14300,57 +14362,52 @@
         <v>21</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="22"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="18"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="18"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="24"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -14365,13 +14422,12 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="19"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="21"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14380,36 +14436,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="18.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="16" style="16" customWidth="1"/>
-    <col min="5" max="5" width="18" style="16" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="7.7109375" style="60" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="59" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" style="59" customWidth="1"/>
+    <col min="4" max="8" width="16.140625" style="59" customWidth="1"/>
+    <col min="9" max="9" width="0" style="59" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="59" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -14435,38 +14488,38 @@
         <v>24</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="55"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="56"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="62"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="H6" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14482,22 +14535,22 @@
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="33"/>
-    <col min="4" max="34" width="10.140625" style="33" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="33"/>
+    <col min="1" max="1" width="14.7109375" style="31" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="31"/>
+    <col min="4" max="34" width="10.140625" style="31" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
-      <c r="C1" s="27"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
@@ -14530,153 +14583,153 @@
       <c r="AG1" s="16"/>
       <c r="AH1" s="16"/>
     </row>
-    <row r="2" spans="1:34" s="35" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:34" s="33" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>34</v>
+      <c r="B2" s="23" t="s">
+        <v>33</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
     </row>
-    <row r="3" spans="1:34" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="30"/>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
+    <row r="3" spans="1:34" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
     </row>
-    <row r="4" spans="1:34" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
+    <row r="4" spans="1:34" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="26"/>
+      <c r="AH4" s="26"/>
     </row>
-    <row r="5" spans="1:34" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="31"/>
-      <c r="AD5" s="31"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="31"/>
-      <c r="AG5" s="31"/>
-      <c r="AH5" s="31"/>
+    <row r="5" spans="1:34" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>